<commit_message>
FINAL UPDATE (if project not have errors ^-^)
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,84 +16,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>KODE BARANG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>NAMA BARANG</t>
   </si>
   <si>
-    <t>NAMA KATEGORI</t>
-  </si>
-  <si>
-    <t>KONDISI BARANG</t>
-  </si>
-  <si>
-    <t>NOMOR SERIAL</t>
-  </si>
-  <si>
-    <t>NOMOR PRODUK</t>
-  </si>
-  <si>
-    <t>KETERANGAN BARANG</t>
-  </si>
-  <si>
-    <t>BATAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAMA SATUAN </t>
-  </si>
-  <si>
-    <t>PHOTO</t>
+    <t>JUMLAH</t>
+  </si>
+  <si>
+    <t>LOKASI</t>
+  </si>
+  <si>
+    <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>USER_SESSION</t>
+  </si>
+  <si>
+    <t>DATEOUT</t>
+  </si>
+  <si>
+    <t>DIVISI</t>
+  </si>
+  <si>
+    <t>NO SURAT JALAN</t>
+  </si>
+  <si>
+    <t>NO LAST SURAT JALAN</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>aaaa</t>
-  </si>
-  <si>
-    <t>Baik</t>
-  </si>
-  <si>
-    <t>aa11</t>
-  </si>
-  <si>
-    <t>11aa</t>
-  </si>
-  <si>
-    <t>jahsu</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>Buruk</t>
-  </si>
-  <si>
-    <t>bb11</t>
-  </si>
-  <si>
-    <t>11bb</t>
-  </si>
-  <si>
-    <t>jsdkjf</t>
-  </si>
-  <si>
-    <t>asas</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>Penguins.jpg</t>
-  </si>
-  <si>
-    <t>Default.jpg</t>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ga</t>
+  </si>
+  <si>
+    <t>ga/wq/2019/06</t>
   </si>
 </sst>
 </file>
@@ -129,11 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,124 +397,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43689</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
+      <c r="J2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>